<commit_message>
Advanced Task Selenium Automation
</commit_message>
<xml_diff>
--- a/marsframework/marsframework-master/MarsFramework/Files/TestData.xlsx
+++ b/marsframework/marsframework-master/MarsFramework/Files/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
   <si>
     <t>FirstName</t>
   </si>
@@ -54,6 +54,9 @@
     <t>Name</t>
   </si>
   <si>
+    <t>First Name</t>
+  </si>
+  <si>
     <t>http://localhost:5000/</t>
   </si>
   <si>
@@ -64,6 +67,9 @@
   </si>
   <si>
     <t>Tester Wang</t>
+  </si>
+  <si>
+    <t>Tester</t>
   </si>
   <si>
     <t>Availability</t>
@@ -174,9 +180,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -222,6 +228,36 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -229,7 +265,37 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -244,14 +310,46 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -264,98 +362,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -378,25 +384,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -408,145 +546,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -570,21 +576,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -595,6 +586,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -619,11 +619,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -663,10 +669,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -675,16 +681,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -694,115 +700,115 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -837,7 +843,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="10" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="10" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1247,21 +1255,22 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="45.8545454545455" customWidth="1"/>
     <col min="2" max="2" width="27.5727272727273" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="4" width="11.4545454545455" customWidth="1"/>
+    <col min="5" max="5" width="11.2727272727273" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -1274,10 +1283,13 @@
       <c r="D1" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" ht="14.5" spans="1:4">
+      <c r="E1" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" ht="14.5" spans="1:5">
       <c r="A2" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>7</v>
@@ -1286,21 +1298,27 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" ht="14.5" spans="1:5">
+      <c r="A3" s="11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" ht="14.5" spans="1:4">
-      <c r="A3" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>14</v>
+      <c r="B3" s="11" t="s">
+        <v>15</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1355,136 +1373,136 @@
   <sheetData>
     <row r="1" ht="42" customHeight="1" spans="1:25">
       <c r="A1" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H1" s="5"/>
       <c r="I1" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="N1" s="5"/>
       <c r="O1" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="R1" s="5"/>
       <c r="S1" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="T1" s="9"/>
       <c r="U1" s="4" t="s">
         <v>11</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="X1" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Y1" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" ht="57.5" spans="1:25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M2" s="8">
         <v>2005</v>
       </c>
       <c r="N2" s="8"/>
       <c r="O2" s="6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="Q2" s="8">
         <v>2019</v>
       </c>
       <c r="R2" s="8"/>
       <c r="S2" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="T2" s="6"/>
       <c r="U2" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="W2" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="X2" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="3:22">

</xml_diff>